<commit_message>
Added sample sites to test against
</commit_message>
<xml_diff>
--- a/web-scraping/settings/sites.xlsx
+++ b/web-scraping/settings/sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/Documents/training/data-analytics/data-analytics-portfolio/web-scraping/settings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897B2570-46B0-244C-966A-2C1D141C9686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98787A2D-1D72-FC49-B94A-3E959D2F27BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="31480" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>url</t>
   </si>
@@ -28,27 +28,32 @@
     <t>browser_to_use</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>http://localhost</t>
-    </r>
+    <t>firefox</t>
   </si>
   <si>
-    <t>firefox</t>
+    <t>http://127.0.0.1:8000</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>table_class</t>
+  </si>
+  <si>
+    <t>https://www.vgchartz.com/charts/platform_totals/Hardware.php</t>
+  </si>
+  <si>
+    <t>myTable</t>
+  </si>
+  <si>
+    <t>chart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -62,10 +67,21 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <u/>
       <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -87,12 +103,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -108,11 +127,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1244,12 +1273,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.33203125" style="1"/>
@@ -1262,34 +1291,46 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
@@ -1307,7 +1348,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CC76A0A7-0B6E-AC42-B072-9E0E7C455AF8}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{2C9C45DB-BBBD-9446-9684-7235AF39EFFF}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>